<commit_message>
Atualização automática de SAO_JOSE_DO_NORTE.xlsx
</commit_message>
<xml_diff>
--- a/SAO_JOSE_DO_NORTE.xlsx
+++ b/SAO_JOSE_DO_NORTE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA2235D0-FA0B-436F-A212-A56C09CBB65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B515148-51C9-46E1-8056-43D721FE7A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1188,7 +1188,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{F0ACFF03-039D-4989-93B8-2C33EA56D3EF}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{EA524F8D-6B1B-42FB-8B06-30D4E4EDA99C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1218,10 +1218,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF64BDBC-D3D2-45EA-B461-DA9296BB9533}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96C78AAF-3E19-4E5F-B88D-693CAA4B4471}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1259,7 +1259,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BA8050C-A4E2-4C25-92A2-583398861BAB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D917382-5AE4-4B8E-8961-57D0BDB417C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1322,7 +1322,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D45B6C95-0E34-4D39-B6DB-88CD42832AB5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25FF5C01-9666-4FE4-A0F1-9BE05966F7BF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1341,7 +1341,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF485E71-291E-F0E7-AFCC-E5F9DE627BAA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DF3F09B-B668-D35E-7011-7125F8D980A9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1390,7 +1390,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AE4F909-89C8-AE4F-54B9-0F1D7A222CC5}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4172DB6-B335-F3D8-6872-96BCEBC81813}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1409,7 +1409,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03AEEEBC-C840-1997-C308-CE75F98F63BA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51062C25-8F56-64B2-74AA-F71CA40A8FC2}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1440,7 +1440,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EC33513-AAA5-1D25-6769-8DF5C4353996}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC8EEAA7-E3B0-9D73-B7CB-4D4823F142FA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1471,7 +1471,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17ECCD3E-4C21-ABE8-6FD7-84B1B7E24431}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12980F24-CBFB-592F-CDAD-991B9C8BF820}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1514,7 +1514,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEE92590-606B-4397-9166-8BDDCF312AF4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55ABEE5C-0DDD-47D2-BAD2-CCAC4252347D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1552,7 +1552,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10028E1B-ACFD-45D2-A7AE-57BCBC6D2690}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38AD4271-E5A3-4D2C-A091-6F1D42693341}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1595,7 +1595,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEA456E1-9A9E-4C55-9068-A7EF803706BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FFC2A65-3101-423F-A66B-3A8537C96257}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1908,7 +1908,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA51D7F-B44C-4E12-8217-72F1F838C2B3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB0F986-0992-477E-923E-901CD85B95C8}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>